<commit_message>
Add risk treatment comparison to standalone site
</commit_message>
<xml_diff>
--- a/standalone/analysis/data/widgetsys.xlsx
+++ b/standalone/analysis/data/widgetsys.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f3a5a03ddb6ab7a/Presentations/SiRAcon 2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agamemnon/GitHub/quantrr/standalone/analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="8_{7096B20E-3056-694E-BC74-EC39EE5177B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7B5A084-8C5F-9D44-B93E-A11D9B7F7967}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6043671-6538-A64D-A7B2-349513BA53F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{48D4EEF9-DFA2-7C44-84E9-995A687A38D6}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="28040" windowHeight="19900" activeTab="2" xr2:uid="{48D4EEF9-DFA2-7C44-84E9-995A687A38D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Risks" sheetId="2" r:id="rId1"/>
-    <sheet name="Estimates" sheetId="1" r:id="rId2"/>
+    <sheet name="Treatments" sheetId="3" r:id="rId2"/>
+    <sheet name="Estimates" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="25">
   <si>
     <t>Expert</t>
   </si>
@@ -97,6 +98,21 @@
   </si>
   <si>
     <t>Risk of losing and existing customer or failure to acquire a new customer due to functional limitations of the inventory system.</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Replace</t>
+  </si>
+  <si>
+    <t>Current system as it is today</t>
+  </si>
+  <si>
+    <t>Replace WMS with a modern solution</t>
   </si>
 </sst>
 </file>
@@ -547,349 +563,834 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408EAE72-3968-D14E-B088-CF815841228E}">
-  <dimension ref="A1:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9314F09A-DCBE-7C4C-8FF0-DDB28C82398C}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="6" width="20.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="100.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{408EAE72-3968-D14E-B088-CF815841228E}">
+  <dimension ref="A1:G43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="7" width="20.83203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>2000</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>45000000</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>300000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>1400</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>34000000</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>200000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>2100</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>54000000</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>500000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.25</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>1900</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>44000000</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>275000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>700</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>200000</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>15000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>500</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="3">
         <v>150000</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>10000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>675</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="3">
         <v>180000</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>11000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>800</v>
       </c>
-      <c r="E15" s="3">
+      <c r="F15" s="3">
         <v>220000</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>16000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>1</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>2</v>
       </c>
-      <c r="D19" s="3">
+      <c r="E19" s="3">
         <v>100000</v>
       </c>
-      <c r="E19" s="3">
+      <c r="F19" s="3">
         <v>20000000</v>
       </c>
-      <c r="F19" s="3">
+      <c r="G19" s="3">
         <v>1500000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>3</v>
       </c>
-      <c r="D20" s="3">
+      <c r="E20" s="3">
         <v>150000</v>
       </c>
-      <c r="E20" s="3">
+      <c r="F20" s="3">
         <v>30000000</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>2000000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>3</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>1</v>
       </c>
-      <c r="D21" s="3">
+      <c r="E21" s="3">
         <v>75000</v>
       </c>
-      <c r="E21" s="3">
+      <c r="F21" s="3">
         <v>15000000</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>1200000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>14</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>7</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>2</v>
       </c>
-      <c r="D22" s="3">
+      <c r="E22" s="3">
         <v>75000</v>
       </c>
-      <c r="E22" s="3">
+      <c r="F22" s="3">
         <v>15000000</v>
       </c>
-      <c r="F22" s="3">
+      <c r="G22" s="3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F26" s="3">
+        <v>45000000</v>
+      </c>
+      <c r="G26" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1400</v>
+      </c>
+      <c r="F27" s="3">
+        <v>34000000</v>
+      </c>
+      <c r="G27" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2100</v>
+      </c>
+      <c r="F28" s="3">
+        <v>54000000</v>
+      </c>
+      <c r="G28" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>0.1</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1900</v>
+      </c>
+      <c r="F29" s="3">
+        <v>44000000</v>
+      </c>
+      <c r="G29" s="3">
+        <v>275000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3">
+        <v>700</v>
+      </c>
+      <c r="F33" s="3">
+        <v>150000</v>
+      </c>
+      <c r="G33" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="3">
+        <v>500</v>
+      </c>
+      <c r="F34" s="3">
+        <v>125000</v>
+      </c>
+      <c r="G34" s="3">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="3">
+        <v>675</v>
+      </c>
+      <c r="F35" s="3">
+        <v>160000</v>
+      </c>
+      <c r="G35" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3">
+        <v>800</v>
+      </c>
+      <c r="F36" s="3">
+        <v>155000</v>
+      </c>
+      <c r="G36" s="3">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0.2</v>
+      </c>
+      <c r="E40" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F40" s="3">
+        <v>20000000</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>0.4</v>
+      </c>
+      <c r="E41" s="3">
+        <v>150000</v>
+      </c>
+      <c r="F41" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="G41" s="3">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>0.25</v>
+      </c>
+      <c r="E42" s="3">
+        <v>75000</v>
+      </c>
+      <c r="F42" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="G42" s="3">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <v>0.1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>75000</v>
+      </c>
+      <c r="F43" s="3">
+        <v>15000000</v>
+      </c>
+      <c r="G43" s="3">
         <v>1000000</v>
       </c>
     </row>

</xml_diff>